<commit_message>
version funcional con GUI
</commit_message>
<xml_diff>
--- a/baseDeDatosParaRevisionDeListas.xlsx
+++ b/baseDeDatosParaRevisionDeListas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\kaht\Proyectos\electroProyects\listasDeChequeo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5E42EA-DE78-422E-8B63-CBB747F64425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D30D6A7-E139-46B7-892F-BF595DA45039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2745" windowWidth="29040" windowHeight="15720" xr2:uid="{53ABC7C9-5DEB-493A-A2AD-94F27270A5B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{53ABC7C9-5DEB-493A-A2AD-94F27270A5B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="190">
   <si>
     <t>ÍTEM</t>
   </si>
@@ -570,31 +570,40 @@
     <t>INS-21-POP</t>
   </si>
   <si>
-    <t>INS-22-BOG</t>
-  </si>
-  <si>
-    <t>INS-23-MED</t>
-  </si>
-  <si>
-    <t>INS-24-CAL</t>
-  </si>
-  <si>
-    <t>INS-25-BAR</t>
-  </si>
-  <si>
-    <t>INS-26-CUC</t>
-  </si>
-  <si>
-    <t>INS-27-CTG</t>
-  </si>
-  <si>
-    <t>INS-28-MAN</t>
-  </si>
-  <si>
-    <t>INS-29-PER</t>
-  </si>
-  <si>
-    <t>INS-30-BUC</t>
+    <t>COMPUTADOR</t>
+  </si>
+  <si>
+    <t>DELL</t>
+  </si>
+  <si>
+    <t>DELL-012</t>
+  </si>
+  <si>
+    <t>INS-21.1-BOG</t>
+  </si>
+  <si>
+    <t>INS-21.2-MED</t>
+  </si>
+  <si>
+    <t>INS-21.3-CAL</t>
+  </si>
+  <si>
+    <t>INS-21.4-BAR</t>
+  </si>
+  <si>
+    <t>INS-21.5-CUC</t>
+  </si>
+  <si>
+    <t>INS-21.6-CTG</t>
+  </si>
+  <si>
+    <t>INS-21.7-MAN</t>
+  </si>
+  <si>
+    <t>INS-21.8-PER</t>
+  </si>
+  <si>
+    <t>INS-21.9-BUC</t>
   </si>
 </sst>
 </file>
@@ -1092,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DF05A2-5B82-4866-AE00-4014001488B4}">
   <dimension ref="A1:AX33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AW31" sqref="AW31"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3623,7 +3632,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:50" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3631,16 +3640,16 @@
         <v>177</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>79</v>
+        <v>179</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>103</v>
+        <v>180</v>
       </c>
       <c r="F22" s="1">
-        <v>901234567</v>
+        <v>132681</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>157</v>
@@ -3649,85 +3658,13 @@
         <v>45512</v>
       </c>
       <c r="I22" s="12">
-        <v>45696</v>
+        <v>45512</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>104</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG22" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="AH22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN22" s="1">
-        <v>59</v>
-      </c>
-      <c r="AO22" s="1">
-        <v>10</v>
-      </c>
-      <c r="AP22" s="1">
-        <v>91</v>
-      </c>
-      <c r="AQ22" s="1">
-        <v>80</v>
-      </c>
-      <c r="AR22" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AS22" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AT22" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AU22" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AV22" s="1" t="s">
-        <v>153</v>
+        <v>56</v>
       </c>
       <c r="AW22" s="1" t="s">
         <v>54</v>
@@ -3741,109 +3678,34 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>71</v>
+        <v>179</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="F23" s="1">
-        <v>123456789</v>
+        <v>6841321</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H23" s="12">
-        <v>45244</v>
+        <v>45512</v>
       </c>
       <c r="I23" s="12">
-        <v>45426</v>
+        <v>45512</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>59</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN23" s="1">
-        <v>50</v>
-      </c>
-      <c r="AO23" s="1">
-        <v>1</v>
-      </c>
-      <c r="AP23" s="1">
-        <v>100</v>
-      </c>
-      <c r="AQ23" s="1">
-        <v>71</v>
-      </c>
-      <c r="AR23" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AS23" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="AT23" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AU23" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AV23" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="AW23" s="1" t="s">
         <v>156</v>
@@ -3857,109 +3719,34 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>75</v>
+        <v>180</v>
       </c>
       <c r="F24" s="1">
-        <v>987654321</v>
+        <v>6843</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H24" s="12">
-        <v>45261</v>
+        <v>45512</v>
       </c>
       <c r="I24" s="12">
-        <v>45444</v>
+        <v>45512</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>76</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="X24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN24" s="1">
-        <v>51</v>
-      </c>
-      <c r="AO24" s="1">
-        <v>2</v>
-      </c>
-      <c r="AP24" s="1">
-        <v>99</v>
-      </c>
-      <c r="AQ24" s="1">
-        <v>72</v>
-      </c>
-      <c r="AR24" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AS24" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AT24" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AU24" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV24" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="AW24" s="1" t="s">
         <v>158</v>
@@ -3973,109 +3760,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="F25" s="1">
-        <v>234567890</v>
+        <v>351</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H25" s="12">
-        <v>45296</v>
+        <v>45512</v>
       </c>
       <c r="I25" s="12">
-        <v>45478</v>
+        <v>45512</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="X25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AN25" s="1">
-        <v>52</v>
-      </c>
-      <c r="AO25" s="1">
-        <v>3</v>
-      </c>
-      <c r="AP25" s="1">
-        <v>98</v>
-      </c>
-      <c r="AQ25" s="1">
-        <v>73</v>
-      </c>
-      <c r="AR25" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AS25" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AT25" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AU25" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AV25" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="AW25" s="1" t="s">
         <v>54</v>
@@ -4089,109 +3801,34 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>178</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="F26" s="1">
-        <v>345678901</v>
+        <v>321</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>157</v>
       </c>
       <c r="H26" s="12">
-        <v>45324</v>
+        <v>45512</v>
       </c>
       <c r="I26" s="12">
-        <v>45506</v>
+        <v>45512</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>61</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="U26" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="V26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN26" s="1">
-        <v>53</v>
-      </c>
-      <c r="AO26" s="1">
-        <v>4</v>
-      </c>
-      <c r="AP26" s="1">
-        <v>97</v>
-      </c>
-      <c r="AQ26" s="1">
-        <v>74</v>
-      </c>
-      <c r="AR26" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AS26" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AT26" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AU26" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AV26" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="AW26" s="1" t="s">
         <v>162</v>
@@ -4205,109 +3842,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>63</v>
+        <v>178</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>85</v>
+        <v>180</v>
       </c>
       <c r="F27" s="1">
-        <v>456789012</v>
+        <v>3541</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H27" s="12">
-        <v>45354</v>
+        <v>45512</v>
       </c>
       <c r="I27" s="12">
-        <v>45538</v>
+        <v>45512</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>86</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="W27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="X27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN27" s="1">
-        <v>54</v>
-      </c>
-      <c r="AO27" s="1">
-        <v>5</v>
-      </c>
-      <c r="AP27" s="1">
-        <v>96</v>
-      </c>
-      <c r="AQ27" s="1">
-        <v>75</v>
-      </c>
-      <c r="AR27" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AS27" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AT27" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AU27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AV27" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="AW27" s="1" t="s">
         <v>159</v>
@@ -4321,109 +3883,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>88</v>
+        <v>178</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>79</v>
+        <v>179</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>89</v>
+        <v>180</v>
       </c>
       <c r="F28" s="1">
-        <v>567890123</v>
+        <v>6354</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H28" s="12">
-        <v>45386</v>
+        <v>45512</v>
       </c>
       <c r="I28" s="12">
-        <v>45569</v>
+        <v>45512</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y28" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AN28" s="1">
-        <v>55</v>
-      </c>
-      <c r="AO28" s="1">
-        <v>6</v>
-      </c>
-      <c r="AP28" s="1">
-        <v>95</v>
-      </c>
-      <c r="AQ28" s="1">
-        <v>76</v>
-      </c>
-      <c r="AR28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AS28" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AT28" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AU28" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AV28" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="AW28" s="1" t="s">
         <v>165</v>
@@ -4437,112 +3924,34 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>66</v>
+        <v>178</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>91</v>
+        <v>179</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="F29" s="1">
-        <v>678901234</v>
+        <v>646</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H29" s="12">
-        <v>45417</v>
+        <v>45512</v>
       </c>
       <c r="I29" s="12">
-        <v>45601</v>
+        <v>45512</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>65</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="V29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA29" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM29" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN29" s="1">
-        <v>56</v>
-      </c>
-      <c r="AO29" s="1">
-        <v>7</v>
-      </c>
-      <c r="AP29" s="1">
-        <v>94</v>
-      </c>
-      <c r="AQ29" s="1">
-        <v>77</v>
-      </c>
-      <c r="AR29" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AS29" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AT29" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AU29" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AV29" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="AW29" s="1" t="s">
         <v>155</v>
@@ -4556,109 +3965,34 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>93</v>
+        <v>178</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>94</v>
+        <v>179</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="F30" s="1">
-        <v>789012345</v>
+        <v>64</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H30" s="12">
-        <v>45449</v>
+        <v>45512</v>
       </c>
       <c r="I30" s="12">
-        <v>45632</v>
+        <v>45512</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>57</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="X30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC30" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AD30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK30" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AL30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN30" s="1">
-        <v>57</v>
-      </c>
-      <c r="AO30" s="1">
-        <v>8</v>
-      </c>
-      <c r="AP30" s="1">
-        <v>93</v>
-      </c>
-      <c r="AQ30" s="1">
-        <v>78</v>
-      </c>
-      <c r="AR30" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AS30" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AT30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AU30" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AV30" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="AW30" s="1" t="s">
         <v>156</v>
@@ -4672,112 +4006,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>97</v>
+        <v>178</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>98</v>
+        <v>179</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>99</v>
+        <v>180</v>
       </c>
       <c r="F31" s="1">
-        <v>890123456</v>
+        <v>684132</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H31" s="12">
-        <v>45480</v>
+        <v>45512</v>
       </c>
       <c r="I31" s="12">
-        <v>45664</v>
+        <v>45512</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>100</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="X31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE31" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AF31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI31" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AJ31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AN31" s="1">
-        <v>58</v>
-      </c>
-      <c r="AO31" s="1">
-        <v>9</v>
-      </c>
-      <c r="AP31" s="1">
-        <v>92</v>
-      </c>
-      <c r="AQ31" s="1">
-        <v>79</v>
-      </c>
-      <c r="AR31" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AS31" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AT31" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AU31" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AV31" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="AW31" s="1" t="s">
         <v>158</v>

</xml_diff>